<commit_message>
Ejercicios 1,2 y 3 listos en PLC
:angel:
</commit_message>
<xml_diff>
--- a/FluidE-S/RELACION E-S.xlsx
+++ b/FluidE-S/RELACION E-S.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\PLC\FluidE-S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F02F01A-3AF2-419C-B5C7-A640E8F01AE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8FEBD3-1BE4-4AF2-BEA6-2F4B201DDD6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{31BB8279-5BB6-4433-890C-37928397B367}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{31BB8279-5BB6-4433-890C-37928397B367}"/>
   </bookViews>
   <sheets>
     <sheet name="Direcciones por ejercicio" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="360">
   <si>
     <t xml:space="preserve">ejercicios </t>
   </si>
@@ -1051,6 +1052,60 @@
   </si>
   <si>
     <t>AB18</t>
+  </si>
+  <si>
+    <t>C_CONTINUO</t>
+  </si>
+  <si>
+    <t>C_UNICO</t>
+  </si>
+  <si>
+    <t>PARO</t>
+  </si>
+  <si>
+    <t>DET_PIEZA</t>
+  </si>
+  <si>
+    <t>N/C</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>C0</t>
+  </si>
+  <si>
+    <t>1Y1</t>
+  </si>
+  <si>
+    <t>1Y2</t>
+  </si>
+  <si>
+    <t>1Y3</t>
+  </si>
+  <si>
+    <t>1Y4</t>
+  </si>
+  <si>
+    <t>1Y5</t>
+  </si>
+  <si>
+    <t>1Y6</t>
+  </si>
+  <si>
+    <t>Entradas</t>
+  </si>
+  <si>
+    <t>Salidas</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1231,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1205,6 +1260,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1531,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873BA327-33BA-4188-8DF7-755A048216E2}">
   <dimension ref="B1:D321"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3307,4 +3368,205 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4479E5A1-3D83-48F1-9389-443073603DD9}">
+  <dimension ref="B3:T6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="10" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="L3" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2">
+        <v>7</v>
+      </c>
+      <c r="N4" s="2">
+        <v>6</v>
+      </c>
+      <c r="O4" s="2">
+        <v>5</v>
+      </c>
+      <c r="P4" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>3</v>
+      </c>
+      <c r="R4" s="2">
+        <v>2</v>
+      </c>
+      <c r="S4" s="2">
+        <v>1</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="L3:T3"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mas cambios de PLC :smile_cat:
:angry:
</commit_message>
<xml_diff>
--- a/FluidE-S/RELACION E-S.xlsx
+++ b/FluidE-S/RELACION E-S.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\PLC\FluidE-S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8FEBD3-1BE4-4AF2-BEA6-2F4B201DDD6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A530BA-A5BC-4CB6-9748-DE980035CDA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{31BB8279-5BB6-4433-890C-37928397B367}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="415">
   <si>
     <t xml:space="preserve">ejercicios </t>
   </si>
@@ -1054,36 +1054,6 @@
     <t>AB18</t>
   </si>
   <si>
-    <t>C_CONTINUO</t>
-  </si>
-  <si>
-    <t>C_UNICO</t>
-  </si>
-  <si>
-    <t>PARO</t>
-  </si>
-  <si>
-    <t>DET_PIEZA</t>
-  </si>
-  <si>
-    <t>N/C</t>
-  </si>
-  <si>
-    <t>A0</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>B0</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>C0</t>
-  </si>
-  <si>
     <t>1Y1</t>
   </si>
   <si>
@@ -1106,6 +1076,201 @@
   </si>
   <si>
     <t>Salidas</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>1B1</t>
+  </si>
+  <si>
+    <t>1A0</t>
+  </si>
+  <si>
+    <t>1A1</t>
+  </si>
+  <si>
+    <t>1B0</t>
+  </si>
+  <si>
+    <t>1C0</t>
+  </si>
+  <si>
+    <t>1C1</t>
+  </si>
+  <si>
+    <t>1HONGO</t>
+  </si>
+  <si>
+    <t>1RESET</t>
+  </si>
+  <si>
+    <t>1C_UNICO</t>
+  </si>
+  <si>
+    <t>1C_CONTINUO</t>
+  </si>
+  <si>
+    <t>1PARO</t>
+  </si>
+  <si>
+    <t>1DET_PIEZA</t>
+  </si>
+  <si>
+    <t>2HONGO</t>
+  </si>
+  <si>
+    <t>2RESET</t>
+  </si>
+  <si>
+    <t>2C_UNICO</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2A0</t>
+  </si>
+  <si>
+    <t>2A1</t>
+  </si>
+  <si>
+    <t>2B0</t>
+  </si>
+  <si>
+    <t>2B1</t>
+  </si>
+  <si>
+    <t>2C0</t>
+  </si>
+  <si>
+    <t>2C1</t>
+  </si>
+  <si>
+    <t>2Y6</t>
+  </si>
+  <si>
+    <t>2Y5</t>
+  </si>
+  <si>
+    <t>2Y4</t>
+  </si>
+  <si>
+    <t>2Y3</t>
+  </si>
+  <si>
+    <t>2Y2</t>
+  </si>
+  <si>
+    <t>2Y1</t>
+  </si>
+  <si>
+    <t>3HONGO</t>
+  </si>
+  <si>
+    <t>3RESET</t>
+  </si>
+  <si>
+    <t>3C_UNICO</t>
+  </si>
+  <si>
+    <t>3A0</t>
+  </si>
+  <si>
+    <t>3A1</t>
+  </si>
+  <si>
+    <t>3B0</t>
+  </si>
+  <si>
+    <t>3B1</t>
+  </si>
+  <si>
+    <t>3C0</t>
+  </si>
+  <si>
+    <t>3C1</t>
+  </si>
+  <si>
+    <t>3Y1</t>
+  </si>
+  <si>
+    <t>3Y2</t>
+  </si>
+  <si>
+    <t>3Y3</t>
+  </si>
+  <si>
+    <t>3Y4</t>
+  </si>
+  <si>
+    <t>3Y5</t>
+  </si>
+  <si>
+    <t>3Y6</t>
+  </si>
+  <si>
+    <t>4HONGO</t>
+  </si>
+  <si>
+    <t>4RESET</t>
+  </si>
+  <si>
+    <t>4C_UNICO</t>
+  </si>
+  <si>
+    <t>4C_CONTINUO</t>
+  </si>
+  <si>
+    <t>4PARO</t>
+  </si>
+  <si>
+    <t>4A0</t>
+  </si>
+  <si>
+    <t>4A1</t>
+  </si>
+  <si>
+    <t>4B0</t>
+  </si>
+  <si>
+    <t>4B1</t>
+  </si>
+  <si>
+    <t>4C0</t>
+  </si>
+  <si>
+    <t>4C1</t>
+  </si>
+  <si>
+    <t>4D0</t>
+  </si>
+  <si>
+    <t>4D1</t>
+  </si>
+  <si>
+    <t>4Y1</t>
+  </si>
+  <si>
+    <t>4Y2</t>
+  </si>
+  <si>
+    <t>4Y3</t>
+  </si>
+  <si>
+    <t>4Y4</t>
+  </si>
+  <si>
+    <t>4Y5</t>
+  </si>
+  <si>
+    <t>4Y6</t>
+  </si>
+  <si>
+    <t>4Y7</t>
+  </si>
+  <si>
+    <t>4Y8</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1367,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1225,13 +1390,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1264,8 +1455,29 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1593,7 +1805,7 @@
   <dimension ref="B1:D321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3372,43 +3584,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4479E5A1-3D83-48F1-9389-443073603DD9}">
-  <dimension ref="B3:T6"/>
+  <dimension ref="B3:AN20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3:AN6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="10" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" customWidth="1"/>
+    <col min="12" max="20" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
-        <v>358</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="L3" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
+    <row r="3" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="L3" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="V3" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="13"/>
+      <c r="AF3" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="AG3" s="13"/>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="13"/>
+      <c r="AJ3" s="13"/>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="13"/>
+      <c r="AM3" s="13"/>
+      <c r="AN3" s="13"/>
+    </row>
+    <row r="4" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="C4" s="2">
         <v>7</v>
       </c>
@@ -3433,7 +3673,9 @@
       <c r="J4" s="2">
         <v>0</v>
       </c>
-      <c r="L4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="M4" s="2">
         <v>7</v>
       </c>
@@ -3458,103 +3700,655 @@
       <c r="T4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V4" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="W4" s="2">
+        <v>7</v>
+      </c>
+      <c r="X4" s="2">
+        <v>6</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>7</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>6</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>5</v>
+      </c>
+      <c r="AJ4" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="P5" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="Q5" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="R5" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="S5" s="12" t="s">
         <v>343</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="T5" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="L5" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>355</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>354</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>353</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="Z5" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="AA5" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="AB5" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="AC5" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="AD5" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="AF5" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG5" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="AH5" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="AI5" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="AJ5" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="AK5" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="AL5" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="AM5" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="AN5" s="18" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="6" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>322</v>
+        <v>356</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
+        <v>352</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="V6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="AC6" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="AD6" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="19"/>
+      <c r="AH6" s="19"/>
+      <c r="AI6" s="19"/>
+      <c r="AJ6" s="19"/>
+      <c r="AK6" s="19"/>
+      <c r="AL6" s="19"/>
+      <c r="AM6" s="19"/>
+      <c r="AN6" s="19"/>
+    </row>
+    <row r="7" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="K7" s="1">
+        <v>2</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="R7" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="S7" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="T7" s="14" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="8" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="K8" s="1">
+        <v>3</v>
+      </c>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+    </row>
+    <row r="9" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="K9" s="1">
+        <v>4</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>393</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>391</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>390</v>
+      </c>
+      <c r="S9" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="10" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="K10" s="1">
+        <v>5</v>
+      </c>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+    </row>
+    <row r="11" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="K11" s="1">
+        <v>6</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="M11" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="N11" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="O11" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="P11" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q11" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="R11" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="S11" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="T11" s="18" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="12" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="K12" s="1">
+        <v>7</v>
+      </c>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+    </row>
+    <row r="13" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20" s="1">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="49">
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="AF3:AN3"/>
+    <mergeCell ref="AF5:AF6"/>
+    <mergeCell ref="AG5:AG6"/>
+    <mergeCell ref="AH5:AH6"/>
+    <mergeCell ref="AI5:AI6"/>
+    <mergeCell ref="AJ5:AJ6"/>
+    <mergeCell ref="AK5:AK6"/>
+    <mergeCell ref="AL5:AL6"/>
+    <mergeCell ref="AM5:AM6"/>
+    <mergeCell ref="AN5:AN6"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="V3:AD3"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
     <mergeCell ref="R5:R6"/>
     <mergeCell ref="S5:S6"/>
     <mergeCell ref="T5:T6"/>
@@ -3567,6 +4361,7 @@
     <mergeCell ref="P5:P6"/>
     <mergeCell ref="Q5:Q6"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Otros dos ejercicios terminados
</commit_message>
<xml_diff>
--- a/FluidE-S/RELACION E-S.xlsx
+++ b/FluidE-S/RELACION E-S.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\PLC\FluidE-S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A530BA-A5BC-4CB6-9748-DE980035CDA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA903D7-9CEE-40B3-A42C-58B27D659557}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{31BB8279-5BB6-4433-890C-37928397B367}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="451">
   <si>
     <t xml:space="preserve">ejercicios </t>
   </si>
@@ -1271,6 +1271,114 @@
   </si>
   <si>
     <t>4Y8</t>
+  </si>
+  <si>
+    <t>5HONGO</t>
+  </si>
+  <si>
+    <t>5RESET</t>
+  </si>
+  <si>
+    <t>5C_UNICO</t>
+  </si>
+  <si>
+    <t>5A0</t>
+  </si>
+  <si>
+    <t>5A1</t>
+  </si>
+  <si>
+    <t>5B0</t>
+  </si>
+  <si>
+    <t>5B1</t>
+  </si>
+  <si>
+    <t>5C0</t>
+  </si>
+  <si>
+    <t>5C1</t>
+  </si>
+  <si>
+    <t>5Y1</t>
+  </si>
+  <si>
+    <t>5Y2</t>
+  </si>
+  <si>
+    <t>5Y3</t>
+  </si>
+  <si>
+    <t>5Y4</t>
+  </si>
+  <si>
+    <t>5Y5</t>
+  </si>
+  <si>
+    <t>5Y6</t>
+  </si>
+  <si>
+    <t>6HONGO</t>
+  </si>
+  <si>
+    <t>6RESET</t>
+  </si>
+  <si>
+    <t>6C_UNICO</t>
+  </si>
+  <si>
+    <t>6C_CONTINUO</t>
+  </si>
+  <si>
+    <t>6PARO</t>
+  </si>
+  <si>
+    <t>6A0</t>
+  </si>
+  <si>
+    <t>6A1</t>
+  </si>
+  <si>
+    <t>6B0</t>
+  </si>
+  <si>
+    <t>6B1</t>
+  </si>
+  <si>
+    <t>6C0</t>
+  </si>
+  <si>
+    <t>6C1</t>
+  </si>
+  <si>
+    <t>6D0</t>
+  </si>
+  <si>
+    <t>6D1</t>
+  </si>
+  <si>
+    <t>6Y1</t>
+  </si>
+  <si>
+    <t>6Y2</t>
+  </si>
+  <si>
+    <t>6Y3</t>
+  </si>
+  <si>
+    <t>6Y4</t>
+  </si>
+  <si>
+    <t>6Y5</t>
+  </si>
+  <si>
+    <t>6Y6</t>
+  </si>
+  <si>
+    <t>6Y7</t>
+  </si>
+  <si>
+    <t>6Y8</t>
   </si>
 </sst>
 </file>
@@ -1313,7 +1421,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1363,6 +1471,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1422,7 +1536,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1455,7 +1569,16 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1467,16 +1590,19 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1805,7 +1931,7 @@
   <dimension ref="B1:D321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3586,8 +3712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4479E5A1-3D83-48F1-9389-443073603DD9}">
   <dimension ref="B3:AN20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3:AN6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3600,50 +3726,50 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="L3" s="13" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="L3" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="V3" s="13" t="s">
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="V3" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="13"/>
-      <c r="AB3" s="13"/>
-      <c r="AC3" s="13"/>
-      <c r="AD3" s="13"/>
-      <c r="AF3" s="13" t="s">
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AF3" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="AG3" s="13"/>
-      <c r="AH3" s="13"/>
-      <c r="AI3" s="13"/>
-      <c r="AJ3" s="13"/>
-      <c r="AK3" s="13"/>
-      <c r="AL3" s="13"/>
-      <c r="AM3" s="13"/>
-      <c r="AN3" s="13"/>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="16"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="16"/>
+      <c r="AM3" s="16"/>
+      <c r="AN3" s="16"/>
     </row>
     <row r="4" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -3786,86 +3912,84 @@
       <c r="K5" s="1">
         <v>0</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="19" t="s">
         <v>321</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="P5" s="19" t="s">
         <v>346</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="S5" s="12" t="s">
+      <c r="S5" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="T5" s="19" t="s">
         <v>342</v>
       </c>
-      <c r="V5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="W5" s="7" t="s">
+      <c r="V5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="X5" s="7" t="s">
+      <c r="Y5" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="Y5" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="Z5" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="AA5" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="AB5" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="AC5" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="AD5" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="AF5" s="18" t="s">
-        <v>326</v>
-      </c>
-      <c r="AG5" s="18" t="s">
-        <v>414</v>
-      </c>
-      <c r="AH5" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="AI5" s="18" t="s">
-        <v>412</v>
-      </c>
-      <c r="AJ5" s="18" t="s">
-        <v>411</v>
-      </c>
-      <c r="AK5" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="AL5" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="AM5" s="18" t="s">
-        <v>408</v>
-      </c>
-      <c r="AN5" s="18" t="s">
-        <v>407</v>
+      <c r="Z5" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="AA5" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="AB5" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="AC5" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD5" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="AF5" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="AG5" s="22" t="s">
+        <v>450</v>
+      </c>
+      <c r="AH5" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="AI5" s="22" t="s">
+        <v>448</v>
+      </c>
+      <c r="AJ5" s="22" t="s">
+        <v>447</v>
+      </c>
+      <c r="AK5" s="22" t="s">
+        <v>446</v>
+      </c>
+      <c r="AL5" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="AM5" s="22" t="s">
+        <v>444</v>
+      </c>
+      <c r="AN5" s="22" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="6" spans="2:40" x14ac:dyDescent="0.25">
@@ -3899,51 +4023,51 @@
       <c r="K6" s="1">
         <v>1</v>
       </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="V6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="Z6" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="AA6" s="7" t="s">
-        <v>402</v>
-      </c>
-      <c r="AB6" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="AC6" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="AF6" s="19"/>
-      <c r="AG6" s="19"/>
-      <c r="AH6" s="19"/>
-      <c r="AI6" s="19"/>
-      <c r="AJ6" s="19"/>
-      <c r="AK6" s="19"/>
-      <c r="AL6" s="19"/>
-      <c r="AM6" s="19"/>
-      <c r="AN6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="V6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="W6" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="X6" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="Z6" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="AA6" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="AB6" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="AC6" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="AD6" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="AF6" s="23"/>
+      <c r="AG6" s="23"/>
+      <c r="AH6" s="23"/>
+      <c r="AI6" s="23"/>
+      <c r="AJ6" s="23"/>
+      <c r="AK6" s="23"/>
+      <c r="AL6" s="23"/>
+      <c r="AM6" s="23"/>
+      <c r="AN6" s="23"/>
     </row>
     <row r="7" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
@@ -3976,31 +4100,31 @@
       <c r="K7" s="1">
         <v>2</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="L7" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="17" t="s">
         <v>366</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="17" t="s">
         <v>366</v>
       </c>
-      <c r="O7" s="14" t="s">
+      <c r="O7" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="P7" s="14" t="s">
+      <c r="P7" s="17" t="s">
         <v>374</v>
       </c>
-      <c r="Q7" s="14" t="s">
+      <c r="Q7" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="R7" s="14" t="s">
+      <c r="R7" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="S7" s="14" t="s">
+      <c r="S7" s="17" t="s">
         <v>377</v>
       </c>
-      <c r="T7" s="14" t="s">
+      <c r="T7" s="17" t="s">
         <v>378</v>
       </c>
     </row>
@@ -4035,15 +4159,15 @@
       <c r="K8" s="1">
         <v>3</v>
       </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
     </row>
     <row r="9" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
@@ -4076,31 +4200,31 @@
       <c r="K9" s="1">
         <v>4</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="L9" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="N9" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="O9" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="Q9" s="16" t="s">
+      <c r="Q9" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="R9" s="16" t="s">
+      <c r="R9" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="S9" s="16" t="s">
+      <c r="S9" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="T9" s="16" t="s">
+      <c r="T9" s="12" t="s">
         <v>388</v>
       </c>
     </row>
@@ -4135,15 +4259,15 @@
       <c r="K10" s="1">
         <v>5</v>
       </c>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
     </row>
     <row r="11" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
@@ -4176,31 +4300,31 @@
       <c r="K11" s="1">
         <v>6</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="M11" s="18" t="s">
+      <c r="M11" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="N11" s="18" t="s">
+      <c r="N11" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="O11" s="18" t="s">
+      <c r="O11" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="P11" s="18" t="s">
+      <c r="P11" s="14" t="s">
         <v>411</v>
       </c>
-      <c r="Q11" s="18" t="s">
+      <c r="Q11" s="14" t="s">
         <v>410</v>
       </c>
-      <c r="R11" s="18" t="s">
+      <c r="R11" s="14" t="s">
         <v>409</v>
       </c>
-      <c r="S11" s="18" t="s">
+      <c r="S11" s="14" t="s">
         <v>408</v>
       </c>
-      <c r="T11" s="18" t="s">
+      <c r="T11" s="14" t="s">
         <v>407</v>
       </c>
     </row>
@@ -4235,47 +4359,213 @@
       <c r="K12" s="1">
         <v>7</v>
       </c>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
     </row>
     <row r="13" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="5" t="s">
         <v>11</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>415</v>
       </c>
       <c r="K13" s="1">
         <v>8</v>
       </c>
+      <c r="L13" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="N13" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="O13" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="P13" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q13" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="R13" s="20" t="s">
+        <v>426</v>
+      </c>
+      <c r="S13" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="T13" s="20" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="14" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="5" t="s">
         <v>12</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>418</v>
       </c>
       <c r="K14" s="1">
         <v>9</v>
       </c>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
     </row>
     <row r="15" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>13</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>430</v>
       </c>
       <c r="K15" s="1">
         <v>10</v>
       </c>
+      <c r="L15" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>450</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="O15" s="22" t="s">
+        <v>448</v>
+      </c>
+      <c r="P15" s="22" t="s">
+        <v>447</v>
+      </c>
+      <c r="Q15" s="22" t="s">
+        <v>446</v>
+      </c>
+      <c r="R15" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="S15" s="22" t="s">
+        <v>444</v>
+      </c>
+      <c r="T15" s="22" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="16" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="B16" s="8" t="s">
         <v>14</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>435</v>
       </c>
       <c r="K16" s="1">
         <v>11</v>
       </c>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
@@ -4310,7 +4600,58 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="67">
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="L3:T3"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="V3:AD3"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="AF3:AN3"/>
+    <mergeCell ref="AF5:AF6"/>
+    <mergeCell ref="AG5:AG6"/>
+    <mergeCell ref="AH5:AH6"/>
+    <mergeCell ref="AI5:AI6"/>
+    <mergeCell ref="AJ5:AJ6"/>
+    <mergeCell ref="AK5:AK6"/>
+    <mergeCell ref="AL5:AL6"/>
+    <mergeCell ref="AM5:AM6"/>
+    <mergeCell ref="AN5:AN6"/>
+    <mergeCell ref="T7:T8"/>
     <mergeCell ref="Q9:Q10"/>
     <mergeCell ref="R9:R10"/>
     <mergeCell ref="S9:S10"/>
@@ -4327,39 +4668,6 @@
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="AF3:AN3"/>
-    <mergeCell ref="AF5:AF6"/>
-    <mergeCell ref="AG5:AG6"/>
-    <mergeCell ref="AH5:AH6"/>
-    <mergeCell ref="AI5:AI6"/>
-    <mergeCell ref="AJ5:AJ6"/>
-    <mergeCell ref="AK5:AK6"/>
-    <mergeCell ref="AL5:AL6"/>
-    <mergeCell ref="AM5:AM6"/>
-    <mergeCell ref="AN5:AN6"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="V3:AD3"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="L3:T3"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="Q5:Q6"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ejercicios 1-6.5 terminados en PLC
Ya estan documentados, faltan 3
</commit_message>
<xml_diff>
--- a/FluidE-S/RELACION E-S.xlsx
+++ b/FluidE-S/RELACION E-S.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\PLC\FluidE-S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9F5EAB-8DF5-4777-8238-3409BBC5E393}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CA4266-E7E9-4BF2-814B-7AA404BB1ECA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{31BB8279-5BB6-4433-890C-37928397B367}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="630">
   <si>
     <t xml:space="preserve">ejercicios </t>
   </si>
@@ -1655,6 +1655,267 @@
   </si>
   <si>
     <t>36Y8</t>
+  </si>
+  <si>
+    <t>37Y8</t>
+  </si>
+  <si>
+    <t>37Y7</t>
+  </si>
+  <si>
+    <t>37Y6</t>
+  </si>
+  <si>
+    <t>37Y5</t>
+  </si>
+  <si>
+    <t>37Y4</t>
+  </si>
+  <si>
+    <t>37Y1</t>
+  </si>
+  <si>
+    <t>37Y2</t>
+  </si>
+  <si>
+    <t>37Y3</t>
+  </si>
+  <si>
+    <t>37HONGO</t>
+  </si>
+  <si>
+    <t>37RESET</t>
+  </si>
+  <si>
+    <t>37C_UNICO</t>
+  </si>
+  <si>
+    <t>37C_CONTINUO</t>
+  </si>
+  <si>
+    <t>37PARO</t>
+  </si>
+  <si>
+    <t>37DET_PIEZA</t>
+  </si>
+  <si>
+    <t>37A0</t>
+  </si>
+  <si>
+    <t>37A1</t>
+  </si>
+  <si>
+    <t>37B0</t>
+  </si>
+  <si>
+    <t>37B1</t>
+  </si>
+  <si>
+    <t>37C0</t>
+  </si>
+  <si>
+    <t>37C1</t>
+  </si>
+  <si>
+    <t>37D0</t>
+  </si>
+  <si>
+    <t>37D1</t>
+  </si>
+  <si>
+    <t>37C2</t>
+  </si>
+  <si>
+    <t>61HONGO</t>
+  </si>
+  <si>
+    <t>61RESET</t>
+  </si>
+  <si>
+    <t>61C_UNICO</t>
+  </si>
+  <si>
+    <t>61A0</t>
+  </si>
+  <si>
+    <t>61A1</t>
+  </si>
+  <si>
+    <t>61B0</t>
+  </si>
+  <si>
+    <t>61B1</t>
+  </si>
+  <si>
+    <t>61Y1</t>
+  </si>
+  <si>
+    <t>61Y2</t>
+  </si>
+  <si>
+    <t>61Y4</t>
+  </si>
+  <si>
+    <t>E29</t>
+  </si>
+  <si>
+    <t>E30</t>
+  </si>
+  <si>
+    <t>E31</t>
+  </si>
+  <si>
+    <t>E32</t>
+  </si>
+  <si>
+    <t>62HONGO</t>
+  </si>
+  <si>
+    <t>62RESET</t>
+  </si>
+  <si>
+    <t>62C_UNICO</t>
+  </si>
+  <si>
+    <t>62A0</t>
+  </si>
+  <si>
+    <t>62A1</t>
+  </si>
+  <si>
+    <t>62B0</t>
+  </si>
+  <si>
+    <t>62B1</t>
+  </si>
+  <si>
+    <t>62Y1</t>
+  </si>
+  <si>
+    <t>62Y2</t>
+  </si>
+  <si>
+    <t>61Y3</t>
+  </si>
+  <si>
+    <t>62Y4</t>
+  </si>
+  <si>
+    <t>62Y5</t>
+  </si>
+  <si>
+    <t>63HONGO</t>
+  </si>
+  <si>
+    <t>63RESET</t>
+  </si>
+  <si>
+    <t>63C_UNICO</t>
+  </si>
+  <si>
+    <t>63C_CONTINUO</t>
+  </si>
+  <si>
+    <t>63PARO</t>
+  </si>
+  <si>
+    <t>63DET_PIEZA</t>
+  </si>
+  <si>
+    <t>63A0</t>
+  </si>
+  <si>
+    <t>63A1</t>
+  </si>
+  <si>
+    <t>63B0</t>
+  </si>
+  <si>
+    <t>63B1</t>
+  </si>
+  <si>
+    <t>63C0</t>
+  </si>
+  <si>
+    <t>63C1</t>
+  </si>
+  <si>
+    <t>63Y1</t>
+  </si>
+  <si>
+    <t>63Y2</t>
+  </si>
+  <si>
+    <t>63Y3</t>
+  </si>
+  <si>
+    <t>63Y4</t>
+  </si>
+  <si>
+    <t>63Y5</t>
+  </si>
+  <si>
+    <t>63Y6</t>
+  </si>
+  <si>
+    <t>E33</t>
+  </si>
+  <si>
+    <t>E34</t>
+  </si>
+  <si>
+    <t>E37</t>
+  </si>
+  <si>
+    <t>E38</t>
+  </si>
+  <si>
+    <t>E36</t>
+  </si>
+  <si>
+    <t>65HONGO</t>
+  </si>
+  <si>
+    <t>65RESET</t>
+  </si>
+  <si>
+    <t>65C_UNICO</t>
+  </si>
+  <si>
+    <t>65A0</t>
+  </si>
+  <si>
+    <t>65A1</t>
+  </si>
+  <si>
+    <t>65B0</t>
+  </si>
+  <si>
+    <t>65B1</t>
+  </si>
+  <si>
+    <t>65C0</t>
+  </si>
+  <si>
+    <t>65C1</t>
+  </si>
+  <si>
+    <t>65Y1</t>
+  </si>
+  <si>
+    <t>65Y2</t>
+  </si>
+  <si>
+    <t>65Y3</t>
+  </si>
+  <si>
+    <t>65Y4</t>
+  </si>
+  <si>
+    <t>65Y5</t>
+  </si>
+  <si>
+    <t>65Y6</t>
   </si>
 </sst>
 </file>
@@ -1875,7 +2136,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1911,10 +2172,55 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1932,52 +2238,16 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2305,8 +2575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873BA327-33BA-4188-8DF7-755A048216E2}">
   <dimension ref="B1:D321"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4085,10 +4355,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4479E5A1-3D83-48F1-9389-443073603DD9}">
-  <dimension ref="B3:AN31"/>
+  <dimension ref="B3:AN43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+    <sheetView tabSelected="1" topLeftCell="K19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3:AN6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4101,50 +4371,50 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="22" t="s">
         <v>348</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="L3" s="26" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="L3" s="22" t="s">
         <v>349</v>
       </c>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="V3" s="26" t="s">
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="V3" s="22" t="s">
         <v>348</v>
       </c>
-      <c r="W3" s="26"/>
-      <c r="X3" s="26"/>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="26"/>
-      <c r="AC3" s="26"/>
-      <c r="AD3" s="26"/>
-      <c r="AF3" s="26" t="s">
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
+      <c r="AF3" s="22" t="s">
         <v>349</v>
       </c>
-      <c r="AG3" s="26"/>
-      <c r="AH3" s="26"/>
-      <c r="AI3" s="26"/>
-      <c r="AJ3" s="26"/>
-      <c r="AK3" s="26"/>
-      <c r="AL3" s="26"/>
-      <c r="AM3" s="26"/>
-      <c r="AN3" s="26"/>
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
+      <c r="AJ3" s="22"/>
+      <c r="AK3" s="22"/>
+      <c r="AL3" s="22"/>
+      <c r="AM3" s="22"/>
+      <c r="AN3" s="22"/>
     </row>
     <row r="4" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -4287,86 +4557,86 @@
       <c r="K5" s="1">
         <v>0</v>
       </c>
-      <c r="L5" s="29" t="s">
+      <c r="L5" s="23" t="s">
         <v>321</v>
       </c>
-      <c r="M5" s="29" t="s">
-        <v>366</v>
-      </c>
-      <c r="N5" s="29" t="s">
-        <v>366</v>
-      </c>
-      <c r="O5" s="29" t="s">
+      <c r="M5" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="O5" s="23" t="s">
         <v>347</v>
       </c>
-      <c r="P5" s="29" t="s">
+      <c r="P5" s="23" t="s">
         <v>346</v>
       </c>
-      <c r="Q5" s="29" t="s">
+      <c r="Q5" s="23" t="s">
         <v>345</v>
       </c>
-      <c r="R5" s="29" t="s">
+      <c r="R5" s="23" t="s">
         <v>344</v>
       </c>
-      <c r="S5" s="29" t="s">
+      <c r="S5" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="T5" s="29" t="s">
+      <c r="T5" s="23" t="s">
         <v>342</v>
       </c>
-      <c r="V5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="W5" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="X5" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="Y5" s="4" t="s">
-        <v>526</v>
-      </c>
-      <c r="Z5" s="4" t="s">
-        <v>525</v>
-      </c>
-      <c r="AA5" s="4" t="s">
-        <v>524</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>523</v>
-      </c>
-      <c r="AC5" s="4" t="s">
-        <v>522</v>
-      </c>
-      <c r="AD5" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="AF5" s="34" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG5" s="34" t="s">
-        <v>542</v>
-      </c>
-      <c r="AH5" s="34" t="s">
-        <v>541</v>
-      </c>
-      <c r="AI5" s="34" t="s">
-        <v>540</v>
-      </c>
-      <c r="AJ5" s="34" t="s">
-        <v>539</v>
-      </c>
-      <c r="AK5" s="34" t="s">
-        <v>538</v>
-      </c>
-      <c r="AL5" s="34" t="s">
-        <v>537</v>
-      </c>
-      <c r="AM5" s="34" t="s">
-        <v>536</v>
-      </c>
-      <c r="AN5" s="34" t="s">
-        <v>535</v>
+      <c r="V5" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="X5" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="Y5" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="Z5" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="AA5" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="AB5" s="9" t="s">
+        <v>617</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="AD5" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="AF5" s="28" t="s">
+        <v>338</v>
+      </c>
+      <c r="AG5" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="AH5" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="AI5" s="28" t="s">
+        <v>629</v>
+      </c>
+      <c r="AJ5" s="28" t="s">
+        <v>628</v>
+      </c>
+      <c r="AK5" s="28" t="s">
+        <v>627</v>
+      </c>
+      <c r="AL5" s="28" t="s">
+        <v>626</v>
+      </c>
+      <c r="AM5" s="28" t="s">
+        <v>625</v>
+      </c>
+      <c r="AN5" s="28" t="s">
+        <v>624</v>
       </c>
     </row>
     <row r="6" spans="2:40" x14ac:dyDescent="0.25">
@@ -4400,51 +4670,51 @@
       <c r="K6" s="1">
         <v>1</v>
       </c>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="V6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="W6" s="4" t="s">
-        <v>534</v>
-      </c>
-      <c r="X6" s="4" t="s">
-        <v>533</v>
-      </c>
-      <c r="Y6" s="4" t="s">
-        <v>532</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>531</v>
-      </c>
-      <c r="AA6" s="4" t="s">
-        <v>530</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>529</v>
-      </c>
-      <c r="AC6" s="4" t="s">
-        <v>528</v>
-      </c>
-      <c r="AD6" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="AF6" s="35"/>
-      <c r="AG6" s="35"/>
-      <c r="AH6" s="35"/>
-      <c r="AI6" s="35"/>
-      <c r="AJ6" s="35"/>
-      <c r="AK6" s="35"/>
-      <c r="AL6" s="35"/>
-      <c r="AM6" s="35"/>
-      <c r="AN6" s="35"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="V6" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="X6" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="Z6" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="AA6" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="AB6" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="AC6" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="AD6" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="AF6" s="29"/>
+      <c r="AG6" s="29"/>
+      <c r="AH6" s="29"/>
+      <c r="AI6" s="29"/>
+      <c r="AJ6" s="29"/>
+      <c r="AK6" s="29"/>
+      <c r="AL6" s="29"/>
+      <c r="AM6" s="29"/>
+      <c r="AN6" s="29"/>
     </row>
     <row r="7" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
@@ -4477,31 +4747,31 @@
       <c r="K7" s="1">
         <v>2</v>
       </c>
-      <c r="L7" s="27" t="s">
+      <c r="L7" s="24" t="s">
         <v>324</v>
       </c>
-      <c r="M7" s="27" t="s">
-        <v>366</v>
-      </c>
-      <c r="N7" s="27" t="s">
-        <v>366</v>
-      </c>
-      <c r="O7" s="27" t="s">
+      <c r="M7" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="O7" s="24" t="s">
         <v>373</v>
       </c>
-      <c r="P7" s="27" t="s">
+      <c r="P7" s="24" t="s">
         <v>374</v>
       </c>
-      <c r="Q7" s="27" t="s">
+      <c r="Q7" s="24" t="s">
         <v>375</v>
       </c>
-      <c r="R7" s="27" t="s">
+      <c r="R7" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="S7" s="27" t="s">
+      <c r="S7" s="24" t="s">
         <v>377</v>
       </c>
-      <c r="T7" s="27" t="s">
+      <c r="T7" s="24" t="s">
         <v>378</v>
       </c>
     </row>
@@ -4536,15 +4806,15 @@
       <c r="K8" s="1">
         <v>3</v>
       </c>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="28"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
     </row>
     <row r="9" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
@@ -4577,31 +4847,31 @@
       <c r="K9" s="1">
         <v>4</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="M9" s="22" t="s">
-        <v>366</v>
-      </c>
-      <c r="N9" s="22" t="s">
-        <v>366</v>
-      </c>
-      <c r="O9" s="22" t="s">
+      <c r="M9" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="N9" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="O9" s="26" t="s">
         <v>393</v>
       </c>
-      <c r="P9" s="22" t="s">
+      <c r="P9" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="Q9" s="22" t="s">
+      <c r="Q9" s="26" t="s">
         <v>391</v>
       </c>
-      <c r="R9" s="22" t="s">
+      <c r="R9" s="26" t="s">
         <v>390</v>
       </c>
-      <c r="S9" s="22" t="s">
+      <c r="S9" s="26" t="s">
         <v>389</v>
       </c>
-      <c r="T9" s="22" t="s">
+      <c r="T9" s="26" t="s">
         <v>388</v>
       </c>
     </row>
@@ -4636,15 +4906,15 @@
       <c r="K10" s="1">
         <v>5</v>
       </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
     </row>
     <row r="11" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
@@ -4677,31 +4947,31 @@
       <c r="K11" s="1">
         <v>6</v>
       </c>
-      <c r="L11" s="24" t="s">
+      <c r="L11" s="18" t="s">
         <v>326</v>
       </c>
-      <c r="M11" s="24" t="s">
+      <c r="M11" s="18" t="s">
         <v>414</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="18" t="s">
         <v>413</v>
       </c>
-      <c r="O11" s="24" t="s">
+      <c r="O11" s="18" t="s">
         <v>412</v>
       </c>
-      <c r="P11" s="24" t="s">
+      <c r="P11" s="18" t="s">
         <v>411</v>
       </c>
-      <c r="Q11" s="24" t="s">
+      <c r="Q11" s="18" t="s">
         <v>410</v>
       </c>
-      <c r="R11" s="24" t="s">
+      <c r="R11" s="18" t="s">
         <v>409</v>
       </c>
-      <c r="S11" s="24" t="s">
+      <c r="S11" s="18" t="s">
         <v>408</v>
       </c>
-      <c r="T11" s="24" t="s">
+      <c r="T11" s="18" t="s">
         <v>407</v>
       </c>
     </row>
@@ -4736,15 +5006,15 @@
       <c r="K12" s="1">
         <v>7</v>
       </c>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
     </row>
     <row r="13" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
@@ -4777,31 +5047,31 @@
       <c r="K13" s="1">
         <v>8</v>
       </c>
-      <c r="L13" s="30" t="s">
+      <c r="L13" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="M13" s="30" t="s">
-        <v>366</v>
-      </c>
-      <c r="N13" s="30" t="s">
-        <v>366</v>
-      </c>
-      <c r="O13" s="30" t="s">
+      <c r="M13" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="O13" s="16" t="s">
         <v>429</v>
       </c>
-      <c r="P13" s="30" t="s">
+      <c r="P13" s="16" t="s">
         <v>428</v>
       </c>
-      <c r="Q13" s="30" t="s">
+      <c r="Q13" s="16" t="s">
         <v>427</v>
       </c>
-      <c r="R13" s="30" t="s">
+      <c r="R13" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="S13" s="30" t="s">
+      <c r="S13" s="16" t="s">
         <v>425</v>
       </c>
-      <c r="T13" s="30" t="s">
+      <c r="T13" s="16" t="s">
         <v>424</v>
       </c>
     </row>
@@ -4836,15 +5106,15 @@
       <c r="K14" s="1">
         <v>9</v>
       </c>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
     </row>
     <row r="15" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -4875,31 +5145,31 @@
       <c r="K15" s="1">
         <v>10</v>
       </c>
-      <c r="L15" s="32" t="s">
+      <c r="L15" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="M15" s="32" t="s">
+      <c r="M15" s="14" t="s">
         <v>450</v>
       </c>
-      <c r="N15" s="32" t="s">
+      <c r="N15" s="14" t="s">
         <v>449</v>
       </c>
-      <c r="O15" s="32" t="s">
+      <c r="O15" s="14" t="s">
         <v>448</v>
       </c>
-      <c r="P15" s="32" t="s">
+      <c r="P15" s="14" t="s">
         <v>447</v>
       </c>
-      <c r="Q15" s="32" t="s">
+      <c r="Q15" s="14" t="s">
         <v>446</v>
       </c>
-      <c r="R15" s="32" t="s">
+      <c r="R15" s="14" t="s">
         <v>445</v>
       </c>
-      <c r="S15" s="32" t="s">
+      <c r="S15" s="14" t="s">
         <v>444</v>
       </c>
-      <c r="T15" s="32" t="s">
+      <c r="T15" s="14" t="s">
         <v>443</v>
       </c>
     </row>
@@ -4934,15 +5204,15 @@
       <c r="K16" s="1">
         <v>11</v>
       </c>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="33"/>
-      <c r="T16" s="33"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
@@ -4975,31 +5245,31 @@
       <c r="K17" s="1">
         <v>12</v>
       </c>
-      <c r="L17" s="20" t="s">
+      <c r="L17" s="28" t="s">
         <v>329</v>
       </c>
-      <c r="M17" s="20" t="s">
-        <v>366</v>
-      </c>
-      <c r="N17" s="20" t="s">
-        <v>366</v>
-      </c>
-      <c r="O17" s="20" t="s">
+      <c r="M17" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="N17" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="O17" s="28" t="s">
         <v>469</v>
       </c>
-      <c r="P17" s="20" t="s">
+      <c r="P17" s="28" t="s">
         <v>456</v>
       </c>
-      <c r="Q17" s="20" t="s">
+      <c r="Q17" s="28" t="s">
         <v>455</v>
       </c>
-      <c r="R17" s="20" t="s">
+      <c r="R17" s="28" t="s">
         <v>454</v>
       </c>
-      <c r="S17" s="20" t="s">
+      <c r="S17" s="28" t="s">
         <v>453</v>
       </c>
-      <c r="T17" s="20" t="s">
+      <c r="T17" s="28" t="s">
         <v>451</v>
       </c>
     </row>
@@ -5034,15 +5304,15 @@
       <c r="K18" s="1">
         <v>13</v>
       </c>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
@@ -5075,31 +5345,31 @@
       <c r="K19" s="1">
         <v>14</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="L19" s="30" t="s">
         <v>330</v>
       </c>
-      <c r="M19" s="15" t="s">
+      <c r="M19" s="30" t="s">
         <v>492</v>
       </c>
-      <c r="N19" s="15" t="s">
+      <c r="N19" s="30" t="s">
         <v>491</v>
       </c>
-      <c r="O19" s="15" t="s">
+      <c r="O19" s="30" t="s">
         <v>490</v>
       </c>
-      <c r="P19" s="15" t="s">
+      <c r="P19" s="30" t="s">
         <v>489</v>
       </c>
-      <c r="Q19" s="15" t="s">
+      <c r="Q19" s="30" t="s">
         <v>488</v>
       </c>
-      <c r="R19" s="15" t="s">
+      <c r="R19" s="30" t="s">
         <v>487</v>
       </c>
-      <c r="S19" s="15" t="s">
+      <c r="S19" s="30" t="s">
         <v>452</v>
       </c>
-      <c r="T19" s="15" t="s">
+      <c r="T19" s="30" t="s">
         <v>486</v>
       </c>
     </row>
@@ -5134,58 +5404,58 @@
       <c r="K20" s="1">
         <v>15</v>
       </c>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>497</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="32" t="s">
         <v>498</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="19"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="34"/>
       <c r="K21" s="1">
         <v>16</v>
       </c>
-      <c r="L21" s="15" t="s">
+      <c r="L21" s="30" t="s">
         <v>331</v>
       </c>
-      <c r="M21" s="15" t="s">
-        <v>366</v>
-      </c>
-      <c r="N21" s="15" t="s">
-        <v>366</v>
-      </c>
-      <c r="O21" s="15" t="s">
-        <v>366</v>
-      </c>
-      <c r="P21" s="15" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q21" s="15" t="s">
+      <c r="M21" s="30" t="s">
+        <v>366</v>
+      </c>
+      <c r="N21" s="30" t="s">
+        <v>366</v>
+      </c>
+      <c r="O21" s="30" t="s">
+        <v>366</v>
+      </c>
+      <c r="P21" s="30" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q21" s="30" t="s">
         <v>496</v>
       </c>
-      <c r="R21" s="15" t="s">
+      <c r="R21" s="30" t="s">
         <v>494</v>
       </c>
-      <c r="S21" s="15" t="s">
+      <c r="S21" s="30" t="s">
         <v>495</v>
       </c>
-      <c r="T21" s="15" t="s">
+      <c r="T21" s="30" t="s">
         <v>493</v>
       </c>
     </row>
@@ -5220,15 +5490,15 @@
       <c r="K22" s="1">
         <v>17</v>
       </c>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="16"/>
-      <c r="S22" s="16"/>
-      <c r="T22" s="16"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
@@ -5261,31 +5531,31 @@
       <c r="K23" s="1">
         <v>18</v>
       </c>
-      <c r="L23" s="13" t="s">
+      <c r="L23" s="35" t="s">
         <v>332</v>
       </c>
-      <c r="M23" s="13" t="s">
+      <c r="M23" s="35" t="s">
         <v>520</v>
       </c>
-      <c r="N23" s="13" t="s">
+      <c r="N23" s="35" t="s">
         <v>519</v>
       </c>
-      <c r="O23" s="13" t="s">
+      <c r="O23" s="35" t="s">
         <v>518</v>
       </c>
-      <c r="P23" s="13" t="s">
+      <c r="P23" s="35" t="s">
         <v>517</v>
       </c>
-      <c r="Q23" s="13" t="s">
+      <c r="Q23" s="35" t="s">
         <v>516</v>
       </c>
-      <c r="R23" s="13" t="s">
+      <c r="R23" s="35" t="s">
         <v>515</v>
       </c>
-      <c r="S23" s="13" t="s">
+      <c r="S23" s="35" t="s">
         <v>514</v>
       </c>
-      <c r="T23" s="13" t="s">
+      <c r="T23" s="35" t="s">
         <v>513</v>
       </c>
     </row>
@@ -5320,15 +5590,15 @@
       <c r="K24" s="1">
         <v>19</v>
       </c>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="36"/>
+      <c r="R24" s="36"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="36"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
@@ -5361,31 +5631,31 @@
       <c r="K25" s="1">
         <v>20</v>
       </c>
-      <c r="L25" s="34" t="s">
+      <c r="L25" s="20" t="s">
         <v>333</v>
       </c>
-      <c r="M25" s="34" t="s">
+      <c r="M25" s="20" t="s">
         <v>542</v>
       </c>
-      <c r="N25" s="34" t="s">
+      <c r="N25" s="20" t="s">
         <v>541</v>
       </c>
-      <c r="O25" s="34" t="s">
+      <c r="O25" s="20" t="s">
         <v>540</v>
       </c>
-      <c r="P25" s="34" t="s">
+      <c r="P25" s="20" t="s">
         <v>539</v>
       </c>
-      <c r="Q25" s="34" t="s">
+      <c r="Q25" s="20" t="s">
         <v>538</v>
       </c>
-      <c r="R25" s="34" t="s">
+      <c r="R25" s="20" t="s">
         <v>537</v>
       </c>
-      <c r="S25" s="34" t="s">
+      <c r="S25" s="20" t="s">
         <v>536</v>
       </c>
-      <c r="T25" s="34" t="s">
+      <c r="T25" s="20" t="s">
         <v>535</v>
       </c>
     </row>
@@ -5420,70 +5690,828 @@
       <c r="K26" s="1">
         <v>21</v>
       </c>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="35"/>
-      <c r="P26" s="35"/>
-      <c r="Q26" s="35"/>
-      <c r="R26" s="35"/>
-      <c r="S26" s="35"/>
-      <c r="T26" s="35"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>551</v>
       </c>
       <c r="K27" s="1">
         <v>22</v>
       </c>
+      <c r="L27" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="M27" s="37" t="s">
+        <v>543</v>
+      </c>
+      <c r="N27" s="37" t="s">
+        <v>544</v>
+      </c>
+      <c r="O27" s="37" t="s">
+        <v>545</v>
+      </c>
+      <c r="P27" s="37" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q27" s="37" t="s">
+        <v>547</v>
+      </c>
+      <c r="R27" s="37" t="s">
+        <v>550</v>
+      </c>
+      <c r="S27" s="37" t="s">
+        <v>549</v>
+      </c>
+      <c r="T27" s="37" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="6" t="s">
         <v>25</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>565</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>557</v>
       </c>
       <c r="K28" s="1">
         <v>23</v>
       </c>
+      <c r="L28" s="37"/>
+      <c r="M28" s="37"/>
+      <c r="N28" s="37"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="37"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="6" t="s">
         <v>26</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>564</v>
       </c>
       <c r="K29" s="1">
         <v>24</v>
       </c>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="37"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="37"/>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="37"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>566</v>
+      </c>
       <c r="K30" s="1">
         <v>25</v>
       </c>
+      <c r="L30" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="M30" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="N30" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="O30" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="P30" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q30" s="18" t="s">
+        <v>575</v>
+      </c>
+      <c r="R30" s="18" t="s">
+        <v>589</v>
+      </c>
+      <c r="S30" s="18" t="s">
+        <v>574</v>
+      </c>
+      <c r="T30" s="18" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>569</v>
+      </c>
       <c r="K31" s="1">
         <v>26</v>
       </c>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="K32" s="1">
+        <v>27</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="M32" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="N32" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="O32" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="P32" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q32" s="16" t="s">
+        <v>591</v>
+      </c>
+      <c r="R32" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="S32" s="16" t="s">
+        <v>588</v>
+      </c>
+      <c r="T32" s="16" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="K33" s="1">
+        <v>28</v>
+      </c>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>597</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>596</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>595</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>592</v>
+      </c>
+      <c r="K34" s="1">
+        <v>29</v>
+      </c>
+      <c r="L34" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="M34" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="N34" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="O34" s="14" t="s">
+        <v>609</v>
+      </c>
+      <c r="P34" s="14" t="s">
+        <v>608</v>
+      </c>
+      <c r="Q34" s="14" t="s">
+        <v>607</v>
+      </c>
+      <c r="R34" s="14" t="s">
+        <v>606</v>
+      </c>
+      <c r="S34" s="14" t="s">
+        <v>605</v>
+      </c>
+      <c r="T34" s="14" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>602</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>600</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>599</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>598</v>
+      </c>
+      <c r="K35" s="1">
+        <v>30</v>
+      </c>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>617</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="K36" s="1">
+        <v>31</v>
+      </c>
+      <c r="L36" s="28" t="s">
+        <v>338</v>
+      </c>
+      <c r="M36" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="N36" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="O36" s="28" t="s">
+        <v>629</v>
+      </c>
+      <c r="P36" s="28" t="s">
+        <v>628</v>
+      </c>
+      <c r="Q36" s="28" t="s">
+        <v>627</v>
+      </c>
+      <c r="R36" s="28" t="s">
+        <v>626</v>
+      </c>
+      <c r="S36" s="28" t="s">
+        <v>625</v>
+      </c>
+      <c r="T36" s="28" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="K37" s="1">
+        <v>32</v>
+      </c>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B38" s="10" t="s">
+        <v>610</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="1">
+        <v>33</v>
+      </c>
+      <c r="L38" s="30" t="s">
+        <v>339</v>
+      </c>
+      <c r="M38" s="30" t="s">
+        <v>366</v>
+      </c>
+      <c r="N38" s="30" t="s">
+        <v>366</v>
+      </c>
+      <c r="O38" s="30"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="30"/>
+      <c r="S38" s="30"/>
+      <c r="T38" s="30"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B39" s="10" t="s">
+        <v>611</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="1">
+        <v>34</v>
+      </c>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="31"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="31"/>
+      <c r="T39" s="31"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B40" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="1">
+        <v>35</v>
+      </c>
+      <c r="L40" s="35" t="s">
+        <v>340</v>
+      </c>
+      <c r="M40" s="35" t="s">
+        <v>366</v>
+      </c>
+      <c r="N40" s="35" t="s">
+        <v>366</v>
+      </c>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="R40" s="35"/>
+      <c r="S40" s="35"/>
+      <c r="T40" s="35"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B41" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="1">
+        <v>36</v>
+      </c>
+      <c r="L41" s="36"/>
+      <c r="M41" s="36"/>
+      <c r="N41" s="36"/>
+      <c r="O41" s="36"/>
+      <c r="P41" s="36"/>
+      <c r="Q41" s="36"/>
+      <c r="R41" s="36"/>
+      <c r="S41" s="36"/>
+      <c r="T41" s="36"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="1">
+        <v>37</v>
+      </c>
+      <c r="L42" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="M42" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="N42" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="20"/>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="38">
+        <v>38</v>
+      </c>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="21"/>
+      <c r="Q43" s="21"/>
+      <c r="R43" s="21"/>
+      <c r="S43" s="21"/>
+      <c r="T43" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="113">
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="R25:R26"/>
-    <mergeCell ref="S25:S26"/>
-    <mergeCell ref="T25:T26"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="T15:T16"/>
+  <mergeCells count="185">
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="N42:N43"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="P42:P43"/>
+    <mergeCell ref="Q42:Q43"/>
+    <mergeCell ref="R42:R43"/>
+    <mergeCell ref="S42:S43"/>
+    <mergeCell ref="T42:T43"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="O40:O41"/>
+    <mergeCell ref="P40:P41"/>
+    <mergeCell ref="Q40:Q41"/>
+    <mergeCell ref="R40:R41"/>
+    <mergeCell ref="S40:S41"/>
+    <mergeCell ref="T40:T41"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="O38:O39"/>
+    <mergeCell ref="P38:P39"/>
+    <mergeCell ref="Q38:Q39"/>
+    <mergeCell ref="R38:R39"/>
+    <mergeCell ref="S38:S39"/>
+    <mergeCell ref="T38:T39"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="O36:O37"/>
+    <mergeCell ref="P36:P37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="R36:R37"/>
+    <mergeCell ref="S36:S37"/>
+    <mergeCell ref="T36:T37"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="R23:R24"/>
+    <mergeCell ref="S23:S24"/>
+    <mergeCell ref="T23:T24"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="R21:R22"/>
+    <mergeCell ref="S21:S22"/>
+    <mergeCell ref="T21:T22"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="S17:S18"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="R19:R20"/>
+    <mergeCell ref="S19:S20"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="AF3:AN3"/>
+    <mergeCell ref="AL5:AL6"/>
+    <mergeCell ref="AM5:AM6"/>
+    <mergeCell ref="AN5:AN6"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="V3:AD3"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="T7:T8"/>
     <mergeCell ref="O13:O14"/>
     <mergeCell ref="P13:P14"/>
     <mergeCell ref="B3:J3"/>
@@ -5507,78 +6535,67 @@
     <mergeCell ref="L13:L14"/>
     <mergeCell ref="M13:M14"/>
     <mergeCell ref="N13:N14"/>
-    <mergeCell ref="V3:AD3"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="AF3:AN3"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="Q30:Q31"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="Q27:Q29"/>
+    <mergeCell ref="P27:P29"/>
+    <mergeCell ref="O27:O29"/>
+    <mergeCell ref="N27:N29"/>
+    <mergeCell ref="M27:M29"/>
+    <mergeCell ref="L27:L29"/>
+    <mergeCell ref="R30:R31"/>
+    <mergeCell ref="S30:S31"/>
+    <mergeCell ref="T30:T31"/>
     <mergeCell ref="AF5:AF6"/>
     <mergeCell ref="AG5:AG6"/>
     <mergeCell ref="AH5:AH6"/>
     <mergeCell ref="AI5:AI6"/>
     <mergeCell ref="AJ5:AJ6"/>
     <mergeCell ref="AK5:AK6"/>
-    <mergeCell ref="AL5:AL6"/>
-    <mergeCell ref="AM5:AM6"/>
-    <mergeCell ref="AN5:AN6"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="T11:T12"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="R17:R18"/>
-    <mergeCell ref="S17:S18"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="R19:R20"/>
-    <mergeCell ref="S19:S20"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="R21:R22"/>
-    <mergeCell ref="S21:S22"/>
-    <mergeCell ref="T21:T22"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O22"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="P23:P24"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="R23:R24"/>
-    <mergeCell ref="S23:S24"/>
-    <mergeCell ref="T23:T24"/>
+    <mergeCell ref="R25:R26"/>
+    <mergeCell ref="S25:S26"/>
+    <mergeCell ref="T25:T26"/>
+    <mergeCell ref="T27:T29"/>
+    <mergeCell ref="S27:S29"/>
+    <mergeCell ref="R27:R29"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="N32:N33"/>
+    <mergeCell ref="O32:O33"/>
+    <mergeCell ref="P32:P33"/>
+    <mergeCell ref="Q32:Q33"/>
+    <mergeCell ref="R32:R33"/>
+    <mergeCell ref="S32:S33"/>
+    <mergeCell ref="T32:T33"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="N34:N35"/>
+    <mergeCell ref="O34:O35"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="Q34:Q35"/>
+    <mergeCell ref="R34:R35"/>
+    <mergeCell ref="S34:S35"/>
+    <mergeCell ref="T34:T35"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>